<commit_message>
added mobile app support
</commit_message>
<xml_diff>
--- a/Tools/Apparatus.xlsx
+++ b/Tools/Apparatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\preparatory\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70C0A79-DF2C-4BE6-95B7-D629269C3D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173D70BB-4E5A-49C7-AD87-15079C256B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,7 +851,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1485,21 +1485,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D48" zoomScale="89" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="13" max="13" width="28.21875" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="28.28515625" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>243</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v xml:space="preserve">243   يوسف عادل حليم </v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>878</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>878   بافلي اديب سمير</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>879</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v xml:space="preserve">879   ميشيل اكرامي حبيب </v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>525</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v xml:space="preserve">525   مارك سامح ابراهيم </v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>830</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>830   فادي بشرى نادي</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>310</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v xml:space="preserve">310   ابانوب عماد جابر </v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>726</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>726   سامح ملاك صابر</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>336</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v xml:space="preserve">336   يوحنا فايز ادوارد </v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>128</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>128   كارلوس شنودة تادرس</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>718</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>718   بيشوي جرجس عيد</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>838</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>838   كيرلس عوني رافت</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>740</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>740   مينا منير امير</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>435</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v xml:space="preserve">435   فادي هاني صموئيل </v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>440</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v xml:space="preserve">440   فيلوباتير عيد اسحق </v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>225</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>113   اوليفر مجدي سمير</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>126</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>129   مارك روماني القمص دوماديوس</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>337</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>133   ميخائيل جرجس محروس</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>231</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v xml:space="preserve">139   انطونيوس باسم وليم </v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L20">
         <v>211</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>211   امير عادل جرجس حنا</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L21">
         <v>254</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>254   بيتر ماهر عزمي</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L22">
         <v>317</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v xml:space="preserve">317   بولا زاخر جرجس </v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L23">
         <v>325</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v xml:space="preserve">325   سمير سامح سمير </v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L24">
         <v>329</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>329   كيرلس جرجس عيسى</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L25">
         <v>334</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v xml:space="preserve">334   ماريو ماجد مهاود </v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L26">
         <v>338</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>338   ميخائيل القس اسحق قسطور</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L27">
         <v>342</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>342   باترك تيسير ادوار</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L28">
         <v>346</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v xml:space="preserve">346   مارتن مجدي جمال </v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L29">
         <v>343</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>343   بيتر فرنسيس منير فرنسيس</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L30">
         <v>438</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v xml:space="preserve">438   فيلوباتير عماد كمال </v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L31">
         <v>444</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v xml:space="preserve">444   ماثيو موسي مكاري </v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L32">
         <v>445</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v xml:space="preserve">445   مارتن ماجد شوقي </v>
       </c>
     </row>
-    <row r="33" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L33">
         <v>880</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v xml:space="preserve">880   نوفير اسامة حنا </v>
       </c>
     </row>
-    <row r="34" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L34">
         <v>610</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>610   فادي عماد موسى</v>
       </c>
     </row>
-    <row r="35" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L35">
         <v>611</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>611   رضا صبحي ايوب</v>
       </c>
     </row>
-    <row r="36" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L36">
         <v>612</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>612   كيرلس صبحي ايوب</v>
       </c>
     </row>
-    <row r="37" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L37">
         <v>616</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>616   توماس مرزق يوسف</v>
       </c>
     </row>
-    <row r="38" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L38">
         <v>617</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>617   شنودة مرزق يوسف</v>
       </c>
     </row>
-    <row r="39" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L39">
         <v>710</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v xml:space="preserve">710   ابانوب إيهاب سعد </v>
       </c>
     </row>
-    <row r="40" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L40">
         <v>721</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>721   جاستن مجدي ابراهيم توفيق</v>
       </c>
     </row>
-    <row r="41" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L41">
         <v>722</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v xml:space="preserve">722   جون روماني مسعد </v>
       </c>
     </row>
-    <row r="42" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L42">
         <v>735</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>735   مارك منير كامل</v>
       </c>
     </row>
-    <row r="43" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L43">
         <v>812</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>812   فادي نصر رمزي</v>
       </c>
     </row>
-    <row r="44" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L44">
         <v>817</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>817   بيشوي ايمن عبد الروؤف</v>
       </c>
     </row>
-    <row r="45" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L45">
         <v>856</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v xml:space="preserve">856   مينا مدحت سمير </v>
       </c>
     </row>
-    <row r="46" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L46">
         <v>862</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v xml:space="preserve">862   يوسف بولا جميل </v>
       </c>
     </row>
-    <row r="47" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L47">
         <v>865</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>865   كيرلس هاني فوزي</v>
       </c>
     </row>
-    <row r="48" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L48">
         <v>869</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>869   يوسف نشات رزق الله</v>
       </c>
     </row>
-    <row r="49" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L49">
         <v>882</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v xml:space="preserve">882   فرانك عصام جرجس </v>
       </c>
     </row>
-    <row r="50" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L50">
         <v>883</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>883   جورج نشات جورج</v>
       </c>
     </row>
-    <row r="51" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L51">
         <v>889</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>889   يوسف مسامح يوسف</v>
       </c>
     </row>
-    <row r="52" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L52">
         <v>891</v>
       </c>
@@ -2353,16 +2353,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26564200-F093-4A51-857E-5F071A182D00}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView zoomScale="83" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="83" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>425</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>450</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>436</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>433</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>246</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>247</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>248</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>214</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>245</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>519</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>138</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>323</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>318</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>742</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>745</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>738</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>717</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>742</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>866</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>874</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>864</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
         <v>440</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>435</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>231</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>225</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
         <v>243</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
         <v>231</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>511</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>525</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
         <v>525</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
         <v>128</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
         <v>126</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
         <v>310</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
         <v>337</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
         <v>336</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>740</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="36">
         <v>726</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="36">
         <v>718</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
         <v>740</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <v>879</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="36">
         <v>879</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="36">
         <v>830</v>
       </c>
@@ -2774,14 +2774,14 @@
       <selection activeCell="A2" sqref="A2:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="1" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>113</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>0.5493055555555556</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>129</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>133</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0.5493055555555556</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>139</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>211</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>254</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>0.40138888888888891</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>317</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>325</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>329</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>334</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>338</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>342</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>346</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>418</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>438</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>444</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>445</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>530</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>610</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>611</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>612</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>616</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>617</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>710</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>721</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <v>722</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>735</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>812</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>817</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>856</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>862</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>865</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>869</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="31">
         <v>882</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>0.5493055555555556</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>883</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>889</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>891</v>
       </c>
@@ -3427,19 +3427,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3448,7 +3448,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
@@ -3458,7 +3458,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="25"/>
       <c r="C43" s="25"/>
@@ -3468,7 +3468,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
       <c r="B44" s="25"/>
       <c r="C44" s="25"/>
@@ -3478,7 +3478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19"/>
@@ -3502,13 +3502,13 @@
       <selection activeCell="A2" sqref="A2:A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>120</v>
       </c>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
         <v>126</v>
       </c>
@@ -3546,7 +3546,7 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
         <v>128</v>
       </c>
@@ -3559,7 +3559,7 @@
       </c>
       <c r="E4" s="15"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>138</v>
       </c>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>139</v>
       </c>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>214</v>
       </c>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>225</v>
       </c>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>231</v>
       </c>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>231</v>
       </c>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>243</v>
       </c>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>245</v>
       </c>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>246</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>247</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>248</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>310</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>317</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>318</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>323</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>325</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>329</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>336</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>337</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>425</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>433</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>435</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>436</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
         <v>440</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>444</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>445</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
         <v>445</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>450</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>511</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>519</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>525</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
         <v>525</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>616</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>717</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="36">
         <v>718</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
         <v>721</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <v>722</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="36">
         <v>726</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <v>735</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <v>738</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <v>740</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="36">
         <v>740</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <v>742</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="36">
         <v>742</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <v>745</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="36">
         <v>830</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <v>856</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="36">
         <v>856</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="36">
         <v>864</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
         <v>866</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <v>874</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <v>879</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="36">
         <v>879</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <v>883</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <v>891</v>
       </c>
@@ -4228,38 +4228,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="36"/>
       <c r="B60" s="16"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="36"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="36"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="36"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="36"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="36"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="36"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="36"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="36"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="36"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="37"/>
     </row>
   </sheetData>
@@ -4279,9 +4279,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>300</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>400</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>500</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>600</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>700</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>800</v>
       </c>

</xml_diff>